<commit_message>
reportgenerator cli 로 legacy report 생성할 경우, $SCAN_DAST$ 포맷 (On 2024. 2. 14.,) 과 AWB 로 legacy report 생성할 경우, $SCAN_DAST$ 포맷(On Feb 14, 2024,) 모두 parsing 되도록 보완
KST 포맷으로 scan 일자 출력 (레포트의 $SCAN_DATE$와 레포트 현재 시간 기준으로 date 문자열 생성)
</commit_message>
<xml_diff>
--- a/FortifyLoginProject_Security_Report.xlsx
+++ b/FortifyLoginProject_Security_Report.xlsx
@@ -140,7 +140,7 @@
     <t>2FC7D1FF-11E4-468E-B7AB-F127828F4016</t>
   </si>
   <si>
-    <t>2024-02-13</t>
+    <t>Tue Feb 13 20:18:45 KST 2024</t>
   </si>
   <si>
     <t xml:space="preserve">    &lt;span&gt;兀��뤇: &lt;input onmouseout = "UserCheck()" id="User" type="text" name="LoginUser" &gt;&lt;/input&gt;&lt;p id="2"&gt;&lt;/p&gt;&lt;br/&gt;&lt;br/&gt;&lt;/span&gt;
@@ -1453,7 +1453,7 @@
     <col min="22" max="22" hidden="false" width="10.296875" customWidth="true" bestFit="true"/>
     <col min="23" max="23" hidden="false" width="11.4140625" customWidth="true" bestFit="true"/>
     <col min="24" max="24" hidden="false" width="10.296875" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" hidden="false" width="11.3046875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" hidden="false" width="27.890625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>